<commit_message>
Add more standard colors and dysplay applications
</commit_message>
<xml_diff>
--- a/Viewsonic VP2785-4K MCCS codes.xlsx
+++ b/Viewsonic VP2785-4K MCCS codes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>1D</t>
   </si>
@@ -35,9 +35,6 @@
     <t>E9</t>
   </si>
   <si>
-    <t>EA</t>
-  </si>
-  <si>
     <t>DC</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Presence sensor</t>
   </si>
   <si>
-    <t>Gamma</t>
-  </si>
-  <si>
     <t>PIP Position</t>
   </si>
   <si>
@@ -78,10 +72,6 @@
   </si>
   <si>
     <t>Uniformity</t>
-  </si>
-  <si>
-    <t>14 - Adobe
-255 - Custom</t>
   </si>
   <si>
     <t>1 - On
@@ -136,10 +126,6 @@
     <t>Display Application</t>
   </si>
   <si>
-    <t>0 - Default
-3 - Movie</t>
-  </si>
-  <si>
     <t>8D</t>
   </si>
   <si>
@@ -175,22 +161,6 @@
   </si>
   <si>
     <t>Video Input</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>PIP Video Input</t>
-  </si>
-  <si>
-    <t>EF</t>
-  </si>
-  <si>
-    <t>0 - Mini DP
-2 - DisplayPort</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>0 - N/A
@@ -201,11 +171,44 @@
 23 - Type C</t>
   </si>
   <si>
-    <t>3909 - HDMI1
-3904 - HDMI2
-? - DisplayPort
-? - Mini DP
-3913 - Type C</t>
+    <t>1 - sRGB
+2 - 
+4 - 
+5 - 
+6 - 
+8 - 
+11 - 
+14 - Adobe
+15 - EBU
+16 - SMPTE-C
+17 - REC709
+18 - DICOM SIM
+19 - DCI-P3
+21 - CAL 1
+22 - CAL 2
+23 - CAL 3
+24 - iPhone (DCI-P3)
+255 - Custom</t>
+  </si>
+  <si>
+    <t>0 - Default
+3 - Movie
+4 - ?
+48 - Game FPS1
+49 - Game FPS2
+50 - Game RTS
+51 - Game MODA
+52 - Web
+53 - Text
+54 - MAC
+55 - Designer CAD/CAM
+56 - Designer Animation
+57 - Designer VideoEdit
+58 - Photographer Retro
+59 - Photographer Photo
+60 - Photographer Landscape
+61 - Photographer Portrait
+62 - Photographer Monochrome</t>
   </si>
 </sst>
 </file>
@@ -306,8 +309,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A2:D22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A2:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A2:D18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D18"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Code" dataDxfId="3"/>
     <tableColumn id="2" name="Name" dataDxfId="2"/>
@@ -581,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,21 +601,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -620,27 +623,27 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="261" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -648,13 +651,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -662,13 +665,13 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -676,13 +679,13 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -690,13 +693,13 @@
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -704,13 +707,13 @@
         <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -718,13 +721,13 @@
         <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -732,13 +735,13 @@
         <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -746,144 +749,97 @@
         <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>96</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>72</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>97</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="261" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>